<commit_message>
v5 with 100/220 ohms
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/fr_a4_t4_e4_g4b_t4a.xlsx
+++ b/myESC-Particle-DEV/saves/fr_a4_t4_e4_g4b_t4a.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\210023782\Documents\GitHub\ESC\myESC-Particle-DEV\saves\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5040" windowWidth="24030" windowHeight="5100" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="5040" windowWidth="24030" windowHeight="5100" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="d_16_6_4" sheetId="1" r:id="rId1"/>
@@ -126,7 +131,7 @@
     <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -214,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -762,12 +767,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -791,7 +799,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>fr_16_1</a:t>
+              <a:t>fr_16_4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1003,6 +1011,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-56E5-4BEE-A91C-EF2FB86D748D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1185,6 +1198,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-56E5-4BEE-A91C-EF2FB86D748D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1382,6 +1400,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-56E5-4BEE-A91C-EF2FB86D748D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1565,6 +1588,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-56E5-4BEE-A91C-EF2FB86D748D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1602,7 +1630,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1693,7 +1720,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1717,7 +1744,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>fr_25_1</a:t>
+              <a:t>fr_25_4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1929,6 +1956,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A53D-4A69-AE0E-2E17B9E21C63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2111,6 +2143,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A53D-4A69-AE0E-2E17B9E21C63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2308,6 +2345,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A53D-4A69-AE0E-2E17B9E21C63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2491,6 +2533,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A53D-4A69-AE0E-2E17B9E21C63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2528,7 +2575,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2619,7 +2665,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2643,7 +2689,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>fr_25_1</a:t>
+              <a:t>fr_25_4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2855,6 +2901,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0064-47E1-AFAA-2F8921F206DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3037,6 +3088,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0064-47E1-AFAA-2F8921F206DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3234,6 +3290,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0064-47E1-AFAA-2F8921F206DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3417,6 +3478,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0064-47E1-AFAA-2F8921F206DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3454,7 +3520,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3545,7 +3610,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3569,7 +3634,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>fr_25_1</a:t>
+              <a:t>fr_25_4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3781,6 +3846,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7BE-463D-B621-3899C92A7D3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3963,6 +4033,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D7BE-463D-B621-3899C92A7D3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4160,6 +4235,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D7BE-463D-B621-3899C92A7D3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -4343,6 +4423,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D7BE-463D-B621-3899C92A7D3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4380,7 +4465,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4487,7 +4571,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4518,7 +4608,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="fr_16_4!$V$4">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A517C48-2963-43F1-8E2F-DDEECAC7835C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -4569,7 +4665,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4602,7 +4704,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="fr_25_4!$V$4">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A7CD2EB-1DF2-4746-B34B-D901B26BFF51}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -4653,7 +4761,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4686,7 +4800,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="fr_48_4!$V$4">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD910E4-56E2-455A-9525-F65520CAEC88}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -4737,7 +4857,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4770,7 +4896,13 @@
     </cdr:to>
     <cdr:sp macro="" textlink="fr_62_4!$V$4">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F703DC79-C173-49DC-BE9B-53CF3AE8954F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
@@ -4847,7 +4979,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4880,9 +5012,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4915,6 +5064,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10738,8 +10904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12680,8 +12846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E24"/>
+    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14613,8 +14779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="Q4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16537,8 +16703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>